<commit_message>
Camera App functionality and hours logged
Updated log for hours worked. Finished simple functionality for Camera
Tool.
</commit_message>
<xml_diff>
--- a/CapstoneHoursLog.xlsx
+++ b/CapstoneHoursLog.xlsx
@@ -410,7 +410,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,7 +449,9 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4">
+        <v>5</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -463,7 +465,9 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4">
+        <v>1.5</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -549,7 +553,7 @@
       </c>
       <c r="B9" s="3">
         <f>B2+B3+B4+B5+B6+B7+B8</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ref="C9:J9" si="0">C2+C3+C4+C5+C6+C7+C8</f>

</xml_diff>

<commit_message>
Created Bitmap Analysis Class
Decided to practice the Decorator pattern on my Bitmap analysis classes.
So the Bitmap analysis classes decorate/modify already decorated
bitmaps.
</commit_message>
<xml_diff>
--- a/CapstoneHoursLog.xlsx
+++ b/CapstoneHoursLog.xlsx
@@ -44,10 +44,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,18 +81,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,18 +99,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,7 +433,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,145 +472,147 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <f>B2+B3+B4+B5+B6+B7+B8</f>
-        <v>10</v>
-      </c>
-      <c r="C9" s="3">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
         <f t="shared" ref="C9:J9" si="0">C2+C3+C4+C5+C6+C7+C8</f>
         <v>0</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Edge Detection and BitmapEX
Downloaded extension library for WriteableBitmap. Finished Edge
Detection tool. Updated hour log.
</commit_message>
<xml_diff>
--- a/CapstoneHoursLog.xlsx
+++ b/CapstoneHoursLog.xlsx
@@ -433,7 +433,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,7 +475,9 @@
       <c r="B2" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <v>5</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -552,7 +554,9 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -566,7 +570,9 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -582,11 +588,11 @@
       </c>
       <c r="B9" s="4">
         <f>B2+B3+B4+B5+B6+B7+B8</f>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" s="4">
         <f t="shared" ref="C9:J9" si="0">C2+C3+C4+C5+C6+C7+C8</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Testing Motion Reading/Update Log
</commit_message>
<xml_diff>
--- a/CapstoneHoursLog.xlsx
+++ b/CapstoneHoursLog.xlsx
@@ -433,7 +433,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,7 +493,9 @@
       <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3">
+        <v>4.5</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -509,7 +511,9 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>2.5</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -592,7 +596,7 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" ref="C9:J9" si="0">C2+C3+C4+C5+C6+C7+C8</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Finished energy renewal process for animals
Fleshed out the process for all animals to eat and absorb energy.
Created variables that determine at what point the animal will search
for favored and unfavored food. Created a variable which determines when
an animal will reproduce.
Removed unecessary code and moved classes around for better
organisation.
</commit_message>
<xml_diff>
--- a/CapstoneHoursLog.xlsx
+++ b/CapstoneHoursLog.xlsx
@@ -433,7 +433,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,7 +478,9 @@
       <c r="C2" s="3">
         <v>7</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <v>9</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -608,7 +610,7 @@
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>

</xml_diff>